<commit_message>
Final submission: Server verified and all Selenium tests passing
</commit_message>
<xml_diff>
--- a/results/Selenium_Final_Report.xlsx
+++ b/results/Selenium_Final_Report.xlsx
@@ -7,39 +7,129 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="ExecutionResults" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="182">
-  <si>
-    <t>Test Case Scenario</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="182">
   <si>
     <t>Test Case ID</t>
   </si>
   <si>
-    <t>Testcase Description</t>
-  </si>
-  <si>
-    <t>Testcase Steps</t>
-  </si>
-  <si>
-    <t>Testdata</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Actual result</t>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>TC_30</t>
+  </si>
+  <si>
     <t>Valid Login</t>
   </si>
   <si>
@@ -130,96 +220,6 @@
     <t>Final Valid User</t>
   </si>
   <si>
-    <t>TC_01</t>
-  </si>
-  <si>
-    <t>TC_02</t>
-  </si>
-  <si>
-    <t>TC_03</t>
-  </si>
-  <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>TC_05</t>
-  </si>
-  <si>
-    <t>TC_06</t>
-  </si>
-  <si>
-    <t>TC_07</t>
-  </si>
-  <si>
-    <t>TC_08</t>
-  </si>
-  <si>
-    <t>TC_09</t>
-  </si>
-  <si>
-    <t>TC_10</t>
-  </si>
-  <si>
-    <t>TC_11</t>
-  </si>
-  <si>
-    <t>TC_12</t>
-  </si>
-  <si>
-    <t>TC_13</t>
-  </si>
-  <si>
-    <t>TC_14</t>
-  </si>
-  <si>
-    <t>TC_15</t>
-  </si>
-  <si>
-    <t>TC_16</t>
-  </si>
-  <si>
-    <t>TC_17</t>
-  </si>
-  <si>
-    <t>TC_18</t>
-  </si>
-  <si>
-    <t>TC_19</t>
-  </si>
-  <si>
-    <t>TC_20</t>
-  </si>
-  <si>
-    <t>TC_21</t>
-  </si>
-  <si>
-    <t>TC_22</t>
-  </si>
-  <si>
-    <t>TC_23</t>
-  </si>
-  <si>
-    <t>TC_24</t>
-  </si>
-  <si>
-    <t>TC_25</t>
-  </si>
-  <si>
-    <t>TC_26</t>
-  </si>
-  <si>
-    <t>TC_27</t>
-  </si>
-  <si>
-    <t>TC_28</t>
-  </si>
-  <si>
-    <t>TC_29</t>
-  </si>
-  <si>
-    <t>TC_30</t>
-  </si>
-  <si>
     <t>Verify correct credentials</t>
   </si>
   <si>
@@ -400,94 +400,94 @@
     <t>1. Enter nextgen_user 2. Click Login</t>
   </si>
   <si>
-    <t>U: testuser | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: testuser | P: WrongPass</t>
-  </si>
-  <si>
-    <t>U: UnknownUser | P: Pass123!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U:  | P: </t>
-  </si>
-  <si>
-    <t>U: test user | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: ' OR '1'='1 | P: pass</t>
-  </si>
-  <si>
-    <t>U: AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: user!@# | P: pass</t>
-  </si>
-  <si>
-    <t>U: 12345 | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: TESTUSER | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: admin'-- | P: pass</t>
-  </si>
-  <si>
-    <t>U: admin' # | P: pass</t>
-  </si>
-  <si>
-    <t>U: &lt;script&gt;alert(1)&lt;/script&gt; | P: pass</t>
-  </si>
-  <si>
-    <t>U: testuser | P: BBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBB</t>
-  </si>
-  <si>
-    <t>U: testuser | P: 1</t>
-  </si>
-  <si>
-    <t>U: testuser | P: pass!@#</t>
-  </si>
-  <si>
-    <t>U: 	user | P: pass</t>
-  </si>
-  <si>
-    <t>U: TestUser | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: testuser | P: 12345678</t>
-  </si>
-  <si>
-    <t>U: test.user@site.com | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: testuser | P: Pass 123 !</t>
-  </si>
-  <si>
-    <t>U: TéstÜsér | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: testuser  | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U:  testuser | P: Pass123!</t>
-  </si>
-  <si>
-    <t>U: 12345 | P: 67890</t>
-  </si>
-  <si>
-    <t>U: testuser | P: password</t>
-  </si>
-  <si>
-    <t>U: &lt;b&gt;user&lt;/b&gt; | P: pass</t>
-  </si>
-  <si>
-    <t>U: user%00 | P: pass</t>
-  </si>
-  <si>
-    <t>U: testuser | P: pAsS123!</t>
-  </si>
-  <si>
-    <t>U: nextgen_user | P: Pass123!</t>
+    <t>U:testuser|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:testuser|P:WrongPass</t>
+  </si>
+  <si>
+    <t>U:UnknownUser|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:|P:</t>
+  </si>
+  <si>
+    <t>U:test user|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:' OR '1'='1|P:pass</t>
+  </si>
+  <si>
+    <t>U:AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:user!@#|P:pass</t>
+  </si>
+  <si>
+    <t>U:12345|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:TESTUSER|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:admin'--|P:pass</t>
+  </si>
+  <si>
+    <t>U:admin' #|P:pass</t>
+  </si>
+  <si>
+    <t>U:&lt;script&gt;alert(1)&lt;/script&gt;|P:pass</t>
+  </si>
+  <si>
+    <t>U:testuser|P:BBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBBB</t>
+  </si>
+  <si>
+    <t>U:testuser|P:1</t>
+  </si>
+  <si>
+    <t>U:testuser|P:pass!@#</t>
+  </si>
+  <si>
+    <t>U:	user|P:pass</t>
+  </si>
+  <si>
+    <t>U:TestUser|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:testuser|P:12345678</t>
+  </si>
+  <si>
+    <t>U:test.user@site.com|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:testuser|P:Pass 123 !</t>
+  </si>
+  <si>
+    <t>U:TéstÜsér|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:testuser |P:Pass123!</t>
+  </si>
+  <si>
+    <t>U: testuser|P:Pass123!</t>
+  </si>
+  <si>
+    <t>U:12345|P:67890</t>
+  </si>
+  <si>
+    <t>U:testuser|P:password</t>
+  </si>
+  <si>
+    <t>U:&lt;b&gt;user&lt;/b&gt;|P:pass</t>
+  </si>
+  <si>
+    <t>U:user%00|P:pass</t>
+  </si>
+  <si>
+    <t>U:testuser|P:pAsS123!</t>
+  </si>
+  <si>
+    <t>U:nextgen_user|P:Pass123!</t>
   </si>
   <si>
     <t>Navigation to Dashboard</t>
@@ -583,12 +583,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -620,26 +626,12 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -934,9 +926,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="8" width="25.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -1745,11 +1734,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>